<commit_message>
Correção na atividade de análise de código
</commit_message>
<xml_diff>
--- a/dev-sist/Fatec-DS/Tabelas/Lista_de_Keywords_para_categorizacao.xlsx
+++ b/dev-sist/Fatec-DS/Tabelas/Lista_de_Keywords_para_categorizacao.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\RProjet _workspace\Observatorio_ODS_LN\Tabelas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\RProjet _workspace\Fatec-DS\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9756"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496"/>
   </bookViews>
   <sheets>
     <sheet name="categorias" sheetId="1" r:id="rId1"/>
@@ -3386,14 +3386,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F522"/>
+  <dimension ref="A1:F523"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3425,7 +3425,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>152</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>152</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>182</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>182</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>182</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>182</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>182</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>182</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>182</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>153</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>153</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>154</v>
       </c>
@@ -3558,7 +3558,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>154</v>
       </c>
@@ -3570,7 +3570,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>154</v>
       </c>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>154</v>
       </c>
@@ -3594,7 +3594,7 @@
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>154</v>
       </c>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>154</v>
       </c>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>154</v>
       </c>
@@ -3636,7 +3636,7 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>154</v>
       </c>
@@ -3648,7 +3648,7 @@
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>154</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>154</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>154</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>154</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>154</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>154</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>154</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>154</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>154</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>154</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>154</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>154</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>154</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>154</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>154</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>154</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>154</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>154</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>154</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>154</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>154</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>154</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>183</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>183</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>183</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>183</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>183</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>183</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>183</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>183</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>183</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>183</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>183</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>183</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>183</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>183</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>183</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>183</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>183</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>183</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>155</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>156</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>156</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>156</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>156</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>156</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>156</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>156</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>156</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>156</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>189</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>189</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>189</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>189</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>189</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>189</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>189</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>189</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>189</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>189</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>189</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>189</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>189</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>189</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>189</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>189</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>157</v>
       </c>
@@ -5708,7 +5708,8 @@
       </c>
       <c r="E197" s="5"/>
     </row>
-    <row r="199" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="199" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="3" t="s">
         <v>972</v>
       </c>
@@ -5722,7 +5723,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="3" t="s">
         <v>972</v>
       </c>
@@ -5736,7 +5737,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="201" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="3" t="s">
         <v>972</v>
       </c>
@@ -5750,7 +5751,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="3" t="s">
         <v>972</v>
       </c>
@@ -5764,7 +5765,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="3" t="s">
         <v>972</v>
       </c>
@@ -5778,7 +5779,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="3" t="s">
         <v>972</v>
       </c>
@@ -5792,7 +5793,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="3" t="s">
         <v>972</v>
       </c>
@@ -5806,7 +5807,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="3" t="s">
         <v>972</v>
       </c>
@@ -5820,7 +5821,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="3" t="s">
         <v>972</v>
       </c>
@@ -5834,7 +5835,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="3"/>
       <c r="B208" s="3" t="s">
         <v>953</v>
@@ -5846,7 +5847,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="3"/>
       <c r="B209" s="3" t="s">
         <v>951</v>
@@ -5858,7 +5859,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="3"/>
       <c r="B210" s="3" t="s">
         <v>949</v>
@@ -5870,7 +5871,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="3"/>
       <c r="B211" s="3" t="s">
         <v>947</v>
@@ -5882,7 +5883,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="3"/>
       <c r="B212" s="3" t="s">
         <v>945</v>
@@ -5894,7 +5895,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="3"/>
       <c r="B213" s="3" t="s">
         <v>943</v>
@@ -5906,7 +5907,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="3"/>
       <c r="B214" s="3" t="s">
         <v>941</v>
@@ -5918,7 +5919,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="3"/>
       <c r="B215" s="3" t="s">
         <v>939</v>
@@ -5930,7 +5931,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="3" t="s">
         <v>972</v>
       </c>
@@ -5944,7 +5945,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="3" t="s">
         <v>972</v>
       </c>
@@ -5958,7 +5959,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>182</v>
       </c>
@@ -5972,7 +5973,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="3"/>
       <c r="B219" s="3" t="s">
         <v>932</v>
@@ -5984,7 +5985,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="3"/>
       <c r="B220" s="3" t="s">
         <v>930</v>
@@ -5996,7 +5997,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="3"/>
       <c r="B221" s="3" t="s">
         <v>928</v>
@@ -6008,7 +6009,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="3"/>
       <c r="B222" s="3" t="s">
         <v>926</v>
@@ -6020,7 +6021,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="3"/>
       <c r="B223" s="3" t="s">
         <v>924</v>
@@ -6032,7 +6033,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="3"/>
       <c r="B224" s="3" t="s">
         <v>922</v>
@@ -6044,7 +6045,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="3"/>
       <c r="B225" s="3" t="s">
         <v>920</v>
@@ -6056,7 +6057,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="226" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="3"/>
       <c r="B226" s="3" t="s">
         <v>918</v>
@@ -6068,7 +6069,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="3"/>
       <c r="B227" s="3" t="s">
         <v>916</v>
@@ -6080,7 +6081,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="228" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="3"/>
       <c r="B228" s="3" t="s">
         <v>914</v>
@@ -6092,7 +6093,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="229" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="3"/>
       <c r="B229" s="3" t="s">
         <v>912</v>
@@ -6104,7 +6105,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="230" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="3"/>
       <c r="B230" s="3" t="s">
         <v>910</v>
@@ -6116,7 +6117,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="3"/>
       <c r="B231" s="3" t="s">
         <v>908</v>
@@ -6128,7 +6129,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="3"/>
       <c r="B232" s="3" t="s">
         <v>906</v>
@@ -6140,7 +6141,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="3"/>
       <c r="B233" s="3" t="s">
         <v>904</v>
@@ -6152,7 +6153,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="3"/>
       <c r="B234" s="3" t="s">
         <v>902</v>
@@ -6164,7 +6165,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="3"/>
       <c r="B235" s="3" t="s">
         <v>900</v>
@@ -6176,7 +6177,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="236" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="3"/>
       <c r="B236" s="3" t="s">
         <v>898</v>
@@ -6188,7 +6189,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="3" t="s">
         <v>972</v>
       </c>
@@ -6202,7 +6203,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="3" t="s">
         <v>972</v>
       </c>
@@ -6216,7 +6217,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="239" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="3"/>
       <c r="B239" s="3" t="s">
         <v>892</v>
@@ -6228,7 +6229,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="240" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="3"/>
       <c r="B240" s="3" t="s">
         <v>891</v>
@@ -6240,7 +6241,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="3"/>
       <c r="B241" s="3" t="s">
         <v>889</v>
@@ -6252,7 +6253,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="242" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="3"/>
       <c r="B242" s="3" t="s">
         <v>887</v>
@@ -6264,7 +6265,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="243" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="3"/>
       <c r="B243" s="3" t="s">
         <v>886</v>
@@ -6276,7 +6277,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="244" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="3"/>
       <c r="B244" s="3" t="s">
         <v>884</v>
@@ -6288,7 +6289,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="245" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="3"/>
       <c r="B245" s="3" t="s">
         <v>882</v>
@@ -6300,7 +6301,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="246" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="3" t="s">
         <v>972</v>
       </c>
@@ -6314,7 +6315,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="247" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="3" t="s">
         <v>972</v>
       </c>
@@ -6328,7 +6329,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="248" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="3" t="s">
         <v>972</v>
       </c>
@@ -6342,7 +6343,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="249" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="3" t="s">
         <v>972</v>
       </c>
@@ -6356,7 +6357,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="250" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="3" t="s">
         <v>972</v>
       </c>
@@ -6370,7 +6371,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="251" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="3" t="s">
         <v>972</v>
       </c>
@@ -6384,7 +6385,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="252" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="3" t="s">
         <v>972</v>
       </c>
@@ -6398,7 +6399,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="253" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="3"/>
       <c r="B253" s="3" t="s">
         <v>866</v>
@@ -6410,7 +6411,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="254" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="3" t="s">
         <v>972</v>
       </c>
@@ -6424,7 +6425,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="255" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="3" t="s">
         <v>972</v>
       </c>
@@ -6438,7 +6439,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="256" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="3" t="s">
         <v>972</v>
       </c>
@@ -6452,7 +6453,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="257" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="3" t="s">
         <v>972</v>
       </c>
@@ -6466,7 +6467,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="258" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="3"/>
       <c r="B258" s="3" t="s">
         <v>856</v>
@@ -6478,7 +6479,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="3"/>
       <c r="B259" s="3" t="s">
         <v>854</v>
@@ -6490,7 +6491,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="260" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="3"/>
       <c r="B260" s="3" t="s">
         <v>852</v>
@@ -6502,7 +6503,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="261" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="3"/>
       <c r="B261" s="3" t="s">
         <v>850</v>
@@ -6514,7 +6515,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="262" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" s="3"/>
       <c r="B262" s="3" t="s">
         <v>849</v>
@@ -6526,7 +6527,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="263" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="3"/>
       <c r="B263" s="3" t="s">
         <v>848</v>
@@ -6538,7 +6539,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="264" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="3"/>
       <c r="B264" s="3" t="s">
         <v>846</v>
@@ -6550,7 +6551,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="265" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="3" t="s">
         <v>972</v>
       </c>
@@ -6564,7 +6565,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="266" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="3"/>
       <c r="B266" s="3" t="s">
         <v>842</v>
@@ -6576,7 +6577,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="267" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="3"/>
       <c r="B267" s="3" t="s">
         <v>840</v>
@@ -6588,7 +6589,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="268" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="3"/>
       <c r="B268" s="3" t="s">
         <v>838</v>
@@ -6600,7 +6601,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="269" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="3"/>
       <c r="B269" s="3" t="s">
         <v>836</v>
@@ -6612,7 +6613,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="270" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="3"/>
       <c r="B270" s="3" t="s">
         <v>834</v>
@@ -6624,7 +6625,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="271" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" s="3"/>
       <c r="B271" s="3" t="s">
         <v>832</v>
@@ -6636,7 +6637,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="272" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" s="3"/>
       <c r="B272" s="3" t="s">
         <v>830</v>
@@ -6648,7 +6649,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="273" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="3"/>
       <c r="B273" s="3" t="s">
         <v>828</v>
@@ -6660,7 +6661,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="274" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="3"/>
       <c r="B274" s="3" t="s">
         <v>826</v>
@@ -6672,7 +6673,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="275" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="3" t="s">
         <v>972</v>
       </c>
@@ -6686,7 +6687,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="276" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="3" t="s">
         <v>972</v>
       </c>
@@ -6700,7 +6701,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="277" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" s="3"/>
       <c r="B277" s="3" t="s">
         <v>821</v>
@@ -6712,7 +6713,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="278" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="3" t="s">
         <v>973</v>
       </c>
@@ -6726,7 +6727,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="279" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="3"/>
       <c r="B279" s="3" t="s">
         <v>817</v>
@@ -6738,7 +6739,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="280" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="3"/>
       <c r="B280" s="3" t="s">
         <v>815</v>
@@ -6750,7 +6751,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="281" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="3"/>
       <c r="B281" s="3" t="s">
         <v>813</v>
@@ -6762,7 +6763,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="282" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" s="3"/>
       <c r="B282" s="3" t="s">
         <v>811</v>
@@ -6774,7 +6775,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="283" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" s="3" t="s">
         <v>972</v>
       </c>
@@ -6788,7 +6789,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="284" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" s="3"/>
       <c r="B284" s="3" t="s">
         <v>807</v>
@@ -6800,7 +6801,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="285" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" s="3"/>
       <c r="B285" s="3" t="s">
         <v>805</v>
@@ -6826,7 +6827,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="287" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" s="3" t="s">
         <v>972</v>
       </c>
@@ -6840,7 +6841,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="288" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="3" t="s">
         <v>972</v>
       </c>
@@ -6854,7 +6855,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="289" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" s="3" t="s">
         <v>972</v>
       </c>
@@ -6868,7 +6869,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="290" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" s="3" t="s">
         <v>972</v>
       </c>
@@ -6882,7 +6883,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="291" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" s="3" t="s">
         <v>972</v>
       </c>
@@ -6896,7 +6897,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="292" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" s="3" t="s">
         <v>972</v>
       </c>
@@ -6910,7 +6911,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="293" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="3"/>
       <c r="B293" s="3" t="s">
         <v>790</v>
@@ -6936,7 +6937,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="295" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" s="3" t="s">
         <v>972</v>
       </c>
@@ -6950,7 +6951,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="296" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" s="3"/>
       <c r="B296" s="3" t="s">
         <v>784</v>
@@ -6962,7 +6963,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="297" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A297" s="3"/>
       <c r="B297" s="3" t="s">
         <v>783</v>
@@ -6974,7 +6975,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="298" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A298" s="3"/>
       <c r="B298" s="3" t="s">
         <v>781</v>
@@ -6986,7 +6987,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="299" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A299" s="3"/>
       <c r="B299" s="3" t="s">
         <v>780</v>
@@ -6998,7 +6999,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="300" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" s="3"/>
       <c r="B300" s="3" t="s">
         <v>778</v>
@@ -7010,7 +7011,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="301" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A301" s="3"/>
       <c r="B301" s="3" t="s">
         <v>776</v>
@@ -7022,7 +7023,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="302" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A302" s="3" t="s">
         <v>972</v>
       </c>
@@ -7036,7 +7037,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="303" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" s="3" t="s">
         <v>972</v>
       </c>
@@ -7050,7 +7051,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="304" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" s="3" t="s">
         <v>972</v>
       </c>
@@ -7064,7 +7065,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="305" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" s="3"/>
       <c r="B305" s="3" t="s">
         <v>768</v>
@@ -7076,7 +7077,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="306" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A306" s="3"/>
       <c r="B306" s="3" t="s">
         <v>766</v>
@@ -7088,7 +7089,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="307" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A307" s="3"/>
       <c r="B307" s="3" t="s">
         <v>764</v>
@@ -7100,7 +7101,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" s="3"/>
       <c r="B308" s="3" t="s">
         <v>762</v>
@@ -7112,7 +7113,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="3"/>
       <c r="B309" s="3" t="s">
         <v>760</v>
@@ -7124,7 +7125,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="310" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A310" s="3"/>
       <c r="B310" s="3" t="s">
         <v>758</v>
@@ -7136,7 +7137,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="311" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" s="3"/>
       <c r="B311" s="3" t="s">
         <v>756</v>
@@ -7148,7 +7149,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="312" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A312" s="3"/>
       <c r="B312" s="3" t="s">
         <v>755</v>
@@ -7160,7 +7161,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="313" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A313" s="3"/>
       <c r="B313" s="3" t="s">
         <v>754</v>
@@ -7172,7 +7173,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="314" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A314" s="3" t="s">
         <v>972</v>
       </c>
@@ -7186,7 +7187,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="315" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A315" s="3" t="s">
         <v>972</v>
       </c>
@@ -7200,7 +7201,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="316" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A316" s="3"/>
       <c r="B316" s="3" t="s">
         <v>748</v>
@@ -7212,7 +7213,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="317" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A317" s="3"/>
       <c r="B317" s="3" t="s">
         <v>746</v>
@@ -7224,7 +7225,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="318" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A318" s="3"/>
       <c r="B318" s="3" t="s">
         <v>743</v>
@@ -7236,7 +7237,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="319" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A319" s="3"/>
       <c r="B319" s="3" t="s">
         <v>743</v>
@@ -7248,7 +7249,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="320" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A320" s="3"/>
       <c r="B320" s="3" t="s">
         <v>741</v>
@@ -7260,7 +7261,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="321" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A321" s="3"/>
       <c r="B321" s="3" t="s">
         <v>739</v>
@@ -7272,7 +7273,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="322" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A322" s="3"/>
       <c r="B322" s="3" t="s">
         <v>737</v>
@@ -7284,7 +7285,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="323" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" s="3"/>
       <c r="B323" s="3" t="s">
         <v>735</v>
@@ -7296,7 +7297,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="324" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A324" s="3"/>
       <c r="B324" s="3" t="s">
         <v>733</v>
@@ -7308,7 +7309,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="325" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A325" s="3"/>
       <c r="B325" s="3" t="s">
         <v>731</v>
@@ -7320,7 +7321,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="326" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A326" s="3"/>
       <c r="B326" s="3" t="s">
         <v>730</v>
@@ -7332,7 +7333,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="327" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A327" s="3"/>
       <c r="B327" s="3" t="s">
         <v>728</v>
@@ -7344,7 +7345,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="328" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A328" s="3"/>
       <c r="B328" s="3" t="s">
         <v>726</v>
@@ -7356,7 +7357,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="329" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A329" s="3"/>
       <c r="B329" s="3" t="s">
         <v>724</v>
@@ -7368,7 +7369,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="330" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A330" s="3"/>
       <c r="B330" s="3" t="s">
         <v>722</v>
@@ -7380,7 +7381,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="331" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A331" s="3"/>
       <c r="B331" s="3" t="s">
         <v>720</v>
@@ -7392,7 +7393,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="332" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A332" s="3"/>
       <c r="B332" s="3" t="s">
         <v>719</v>
@@ -7404,7 +7405,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="333" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A333" s="3"/>
       <c r="B333" s="3" t="s">
         <v>717</v>
@@ -7416,7 +7417,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="334" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A334" s="3"/>
       <c r="B334" s="3" t="s">
         <v>716</v>
@@ -7428,7 +7429,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="335" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A335" s="3"/>
       <c r="B335" s="3" t="s">
         <v>714</v>
@@ -7440,7 +7441,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="336" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A336" s="3"/>
       <c r="B336" s="3" t="s">
         <v>712</v>
@@ -7452,7 +7453,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="337" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A337" s="3"/>
       <c r="B337" s="3" t="s">
         <v>710</v>
@@ -7464,7 +7465,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="338" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A338" s="3"/>
       <c r="B338" s="3" t="s">
         <v>708</v>
@@ -7476,7 +7477,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="339" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A339" s="3"/>
       <c r="B339" s="3" t="s">
         <v>707</v>
@@ -7488,7 +7489,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="340" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A340" s="3"/>
       <c r="B340" s="3" t="s">
         <v>705</v>
@@ -7500,7 +7501,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="341" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A341" s="3"/>
       <c r="B341" s="3" t="s">
         <v>703</v>
@@ -7512,7 +7513,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="342" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A342" s="3"/>
       <c r="B342" s="3" t="s">
         <v>701</v>
@@ -7524,7 +7525,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="343" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A343" s="3"/>
       <c r="B343" s="3" t="s">
         <v>699</v>
@@ -7536,7 +7537,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="344" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A344" s="3"/>
       <c r="B344" s="3" t="s">
         <v>697</v>
@@ -7548,7 +7549,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="345" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A345" s="3"/>
       <c r="B345" s="3" t="s">
         <v>695</v>
@@ -7560,7 +7561,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="346" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A346" s="3"/>
       <c r="B346" s="3" t="s">
         <v>693</v>
@@ -7572,7 +7573,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="347" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A347" s="3"/>
       <c r="B347" s="3" t="s">
         <v>691</v>
@@ -7584,7 +7585,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="348" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A348" s="3"/>
       <c r="B348" s="3" t="s">
         <v>689</v>
@@ -7596,7 +7597,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="349" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A349" s="3"/>
       <c r="B349" s="3" t="s">
         <v>687</v>
@@ -7608,7 +7609,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="350" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A350" s="3"/>
       <c r="B350" s="3" t="s">
         <v>685</v>
@@ -7620,7 +7621,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="351" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A351" s="3"/>
       <c r="B351" s="3" t="s">
         <v>683</v>
@@ -7632,7 +7633,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="352" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A352" s="3"/>
       <c r="B352" s="3" t="s">
         <v>682</v>
@@ -7644,7 +7645,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="353" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A353" s="3"/>
       <c r="B353" s="3" t="s">
         <v>680</v>
@@ -7656,7 +7657,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="354" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A354" s="3"/>
       <c r="B354" s="3" t="s">
         <v>678</v>
@@ -7668,7 +7669,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="355" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A355" s="3"/>
       <c r="B355" s="3" t="s">
         <v>676</v>
@@ -7680,7 +7681,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="356" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A356" s="3"/>
       <c r="B356" s="3" t="s">
         <v>674</v>
@@ -7692,7 +7693,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="357" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A357" s="3"/>
       <c r="B357" s="3" t="s">
         <v>672</v>
@@ -7704,7 +7705,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="358" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A358" s="3"/>
       <c r="B358" s="3" t="s">
         <v>670</v>
@@ -7716,7 +7717,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="359" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A359" s="3" t="s">
         <v>973</v>
       </c>
@@ -7730,7 +7731,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="360" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A360" s="3"/>
       <c r="B360" s="3" t="s">
         <v>666</v>
@@ -7742,7 +7743,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="361" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A361" s="3"/>
       <c r="B361" s="3" t="s">
         <v>664</v>
@@ -7754,7 +7755,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="362" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A362" s="3"/>
       <c r="B362" s="3" t="s">
         <v>662</v>
@@ -7766,7 +7767,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="363" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A363" s="3"/>
       <c r="B363" s="3" t="s">
         <v>660</v>
@@ -7778,7 +7779,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="364" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A364" s="3"/>
       <c r="B364" s="3" t="s">
         <v>658</v>
@@ -7790,7 +7791,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="365" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A365" s="3"/>
       <c r="B365" s="3" t="s">
         <v>656</v>
@@ -7802,7 +7803,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="366" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A366" s="3"/>
       <c r="B366" s="3" t="s">
         <v>654</v>
@@ -7814,7 +7815,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="367" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A367" s="3"/>
       <c r="B367" s="3" t="s">
         <v>652</v>
@@ -7826,7 +7827,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="368" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A368" s="3"/>
       <c r="B368" s="3" t="s">
         <v>650</v>
@@ -7838,7 +7839,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="369" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A369" s="3"/>
       <c r="B369" s="3" t="s">
         <v>648</v>
@@ -7850,7 +7851,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="370" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A370" s="1" t="s">
         <v>156</v>
       </c>
@@ -7892,7 +7893,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="373" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A373" s="3"/>
       <c r="B373" s="3" t="s">
         <v>643</v>
@@ -7904,7 +7905,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="374" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A374" s="3"/>
       <c r="B374" s="3" t="s">
         <v>641</v>
@@ -7916,7 +7917,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="375" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A375" s="3"/>
       <c r="B375" s="3" t="s">
         <v>639</v>
@@ -7928,7 +7929,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="376" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A376" s="3"/>
       <c r="B376" s="3" t="s">
         <v>637</v>
@@ -7940,7 +7941,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="377" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A377" s="3"/>
       <c r="B377" s="3" t="s">
         <v>635</v>
@@ -7952,7 +7953,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="378" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A378" s="3"/>
       <c r="B378" s="3" t="s">
         <v>633</v>
@@ -7964,7 +7965,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="379" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A379" s="3"/>
       <c r="B379" s="3" t="s">
         <v>631</v>
@@ -7976,7 +7977,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="380" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A380" s="3"/>
       <c r="B380" s="3" t="s">
         <v>629</v>
@@ -7988,7 +7989,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="381" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A381" s="3"/>
       <c r="B381" s="3" t="s">
         <v>627</v>
@@ -8000,7 +8001,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="382" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A382" s="3"/>
       <c r="B382" s="3" t="s">
         <v>625</v>
@@ -8012,7 +8013,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="383" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A383" s="3"/>
       <c r="B383" s="3" t="s">
         <v>623</v>
@@ -8024,7 +8025,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="384" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A384" s="3"/>
       <c r="B384" s="3" t="s">
         <v>621</v>
@@ -8036,7 +8037,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="385" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A385" s="3"/>
       <c r="B385" s="3" t="s">
         <v>619</v>
@@ -8048,7 +8049,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="386" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A386" s="3"/>
       <c r="B386" s="3" t="s">
         <v>617</v>
@@ -8060,7 +8061,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="387" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A387" s="3"/>
       <c r="B387" s="3" t="s">
         <v>615</v>
@@ -8072,7 +8073,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="388" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A388" s="3" t="s">
         <v>972</v>
       </c>
@@ -8086,7 +8087,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="389" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A389" s="3" t="s">
         <v>972</v>
       </c>
@@ -8100,7 +8101,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="390" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A390" s="3" t="s">
         <v>972</v>
       </c>
@@ -8114,7 +8115,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="391" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A391" s="3"/>
       <c r="B391" s="3" t="s">
         <v>607</v>
@@ -8126,7 +8127,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="392" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A392" s="3"/>
       <c r="B392" s="3" t="s">
         <v>605</v>
@@ -8138,7 +8139,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="393" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A393" s="3" t="s">
         <v>972</v>
       </c>
@@ -8152,7 +8153,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="394" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A394" s="3" t="s">
         <v>972</v>
       </c>
@@ -8166,7 +8167,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="395" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A395" s="1" t="s">
         <v>182</v>
       </c>
@@ -8180,7 +8181,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="396" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A396" s="3"/>
       <c r="B396" s="3" t="s">
         <v>597</v>
@@ -8192,7 +8193,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="397" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A397" s="3"/>
       <c r="B397" s="3" t="s">
         <v>595</v>
@@ -8204,7 +8205,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="398" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A398" s="3"/>
       <c r="B398" s="3" t="s">
         <v>593</v>
@@ -8216,7 +8217,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="399" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A399" s="3" t="s">
         <v>972</v>
       </c>
@@ -8230,7 +8231,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="400" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A400" s="3" t="s">
         <v>972</v>
       </c>
@@ -8244,7 +8245,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="401" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A401" s="3"/>
       <c r="B401" s="3" t="s">
         <v>587</v>
@@ -8256,7 +8257,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="402" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A402" s="3" t="s">
         <v>972</v>
       </c>
@@ -8270,7 +8271,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="403" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A403" s="3"/>
       <c r="B403" s="3" t="s">
         <v>583</v>
@@ -8282,7 +8283,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="404" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A404" s="3"/>
       <c r="B404" s="3" t="s">
         <v>581</v>
@@ -8294,7 +8295,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="405" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A405" s="3" t="s">
         <v>972</v>
       </c>
@@ -8308,7 +8309,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="406" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A406" s="3" t="s">
         <v>972</v>
       </c>
@@ -8322,7 +8323,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="407" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A407" s="3"/>
       <c r="B407" s="3" t="s">
         <v>576</v>
@@ -8334,7 +8335,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="408" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A408" s="3" t="s">
         <v>972</v>
       </c>
@@ -8348,7 +8349,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="409" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A409" s="3"/>
       <c r="B409" s="3" t="s">
         <v>572</v>
@@ -8360,7 +8361,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="410" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A410" s="3" t="s">
         <v>972</v>
       </c>
@@ -8374,7 +8375,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="411" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A411" s="3" t="s">
         <v>972</v>
       </c>
@@ -8388,7 +8389,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="412" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A412" s="3"/>
       <c r="B412" s="3" t="s">
         <v>566</v>
@@ -8400,7 +8401,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="413" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A413" s="3"/>
       <c r="B413" s="3" t="s">
         <v>564</v>
@@ -8412,7 +8413,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="414" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A414" s="3"/>
       <c r="B414" s="3" t="s">
         <v>562</v>
@@ -8424,7 +8425,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="415" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A415" s="3"/>
       <c r="B415" s="3" t="s">
         <v>560</v>
@@ -8436,7 +8437,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="416" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A416" s="3"/>
       <c r="B416" s="3" t="s">
         <v>558</v>
@@ -8448,7 +8449,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="417" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A417" s="3"/>
       <c r="B417" s="3" t="s">
         <v>556</v>
@@ -8460,7 +8461,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="418" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A418" s="3"/>
       <c r="B418" s="3" t="s">
         <v>554</v>
@@ -8472,7 +8473,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="419" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A419" s="3"/>
       <c r="B419" s="3" t="s">
         <v>552</v>
@@ -8484,7 +8485,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="420" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A420" s="3"/>
       <c r="B420" s="3" t="s">
         <v>550</v>
@@ -8496,7 +8497,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="421" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A421" s="3"/>
       <c r="B421" s="3" t="s">
         <v>548</v>
@@ -8508,7 +8509,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="422" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A422" s="3"/>
       <c r="B422" s="3" t="s">
         <v>546</v>
@@ -8520,7 +8521,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="423" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A423" s="3"/>
       <c r="B423" s="3" t="s">
         <v>544</v>
@@ -8532,7 +8533,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="424" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A424" s="3"/>
       <c r="B424" s="3" t="s">
         <v>542</v>
@@ -8544,7 +8545,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="425" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A425" s="3"/>
       <c r="B425" s="3" t="s">
         <v>541</v>
@@ -8556,7 +8557,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="426" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A426" s="3"/>
       <c r="B426" s="3" t="s">
         <v>539</v>
@@ -8568,7 +8569,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="427" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A427" s="3"/>
       <c r="B427" s="3" t="s">
         <v>536</v>
@@ -8580,7 +8581,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="428" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A428" s="3"/>
       <c r="B428" s="3" t="s">
         <v>538</v>
@@ -8592,7 +8593,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="429" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A429" s="3"/>
       <c r="B429" s="3" t="s">
         <v>536</v>
@@ -8604,7 +8605,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="430" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A430" s="3"/>
       <c r="B430" s="3" t="s">
         <v>534</v>
@@ -8616,7 +8617,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="431" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A431" s="3"/>
       <c r="B431" s="3" t="s">
         <v>532</v>
@@ -8628,7 +8629,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="432" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A432" s="3"/>
       <c r="B432" s="3" t="s">
         <v>530</v>
@@ -8640,7 +8641,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="433" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A433" s="3"/>
       <c r="B433" s="3" t="s">
         <v>528</v>
@@ -8652,7 +8653,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="434" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A434" s="3"/>
       <c r="B434" s="3" t="s">
         <v>526</v>
@@ -8664,7 +8665,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="435" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A435" s="3"/>
       <c r="B435" s="3" t="s">
         <v>524</v>
@@ -8676,7 +8677,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="436" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A436" s="3" t="s">
         <v>972</v>
       </c>
@@ -8690,7 +8691,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="437" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A437" s="3" t="s">
         <v>972</v>
       </c>
@@ -8704,7 +8705,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="438" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A438" s="3" t="s">
         <v>972</v>
       </c>
@@ -8718,7 +8719,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="439" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A439" s="3" t="s">
         <v>972</v>
       </c>
@@ -8732,7 +8733,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="440" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A440" s="3"/>
       <c r="B440" s="3" t="s">
         <v>514</v>
@@ -8744,7 +8745,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="441" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A441" s="3"/>
       <c r="B441" s="3" t="s">
         <v>512</v>
@@ -8756,7 +8757,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="442" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A442" s="3"/>
       <c r="B442" s="3" t="s">
         <v>510</v>
@@ -8768,7 +8769,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="443" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A443" s="1" t="s">
         <v>156</v>
       </c>
@@ -8782,7 +8783,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="444" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A444" s="3"/>
       <c r="B444" s="3" t="s">
         <v>506</v>
@@ -8794,7 +8795,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="445" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A445" s="3" t="s">
         <v>972</v>
       </c>
@@ -8808,7 +8809,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="446" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A446" s="3" t="s">
         <v>972</v>
       </c>
@@ -8822,7 +8823,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="447" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A447" s="3"/>
       <c r="B447" s="3" t="s">
         <v>500</v>
@@ -8834,7 +8835,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="448" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A448" s="3" t="s">
         <v>972</v>
       </c>
@@ -8848,7 +8849,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="449" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A449" s="3" t="s">
         <v>972</v>
       </c>
@@ -8862,7 +8863,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="450" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A450" s="3"/>
       <c r="B450" s="3" t="s">
         <v>494</v>
@@ -8874,7 +8875,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="451" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A451" s="3"/>
       <c r="B451" s="3" t="s">
         <v>492</v>
@@ -8886,7 +8887,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="452" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A452" s="3" t="s">
         <v>972</v>
       </c>
@@ -8900,7 +8901,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="453" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A453" s="3" t="s">
         <v>972</v>
       </c>
@@ -8914,7 +8915,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="454" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A454" s="3" t="s">
         <v>972</v>
       </c>
@@ -8928,7 +8929,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="455" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A455" s="3" t="s">
         <v>972</v>
       </c>
@@ -8942,7 +8943,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="456" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A456" s="3" t="s">
         <v>972</v>
       </c>
@@ -8956,7 +8957,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="457" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A457" s="3" t="s">
         <v>972</v>
       </c>
@@ -8970,7 +8971,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="458" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A458" s="3" t="s">
         <v>972</v>
       </c>
@@ -8984,7 +8985,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="459" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A459" s="3" t="s">
         <v>972</v>
       </c>
@@ -8998,7 +8999,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="460" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A460" s="3" t="s">
         <v>972</v>
       </c>
@@ -9012,7 +9013,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="461" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A461" s="3"/>
       <c r="B461" s="3" t="s">
         <v>476</v>
@@ -9024,7 +9025,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="462" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A462" s="3"/>
       <c r="B462" s="3" t="s">
         <v>474</v>
@@ -9036,7 +9037,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="463" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A463" s="3"/>
       <c r="B463" s="3" t="s">
         <v>472</v>
@@ -9048,7 +9049,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="464" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A464" s="3"/>
       <c r="B464" s="3" t="s">
         <v>470</v>
@@ -9060,7 +9061,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="465" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A465" s="3"/>
       <c r="B465" s="3" t="s">
         <v>468</v>
@@ -9072,7 +9073,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="466" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A466" s="3"/>
       <c r="B466" s="3" t="s">
         <v>466</v>
@@ -9084,7 +9085,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="467" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A467" s="3"/>
       <c r="B467" s="3" t="s">
         <v>465</v>
@@ -9096,7 +9097,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="468" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A468" s="3"/>
       <c r="B468" s="3" t="s">
         <v>464</v>
@@ -9108,7 +9109,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="469" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A469" s="3"/>
       <c r="B469" s="3" t="s">
         <v>462</v>
@@ -9120,7 +9121,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="470" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A470" s="3"/>
       <c r="B470" s="3" t="s">
         <v>460</v>
@@ -9132,7 +9133,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="471" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A471" s="3"/>
       <c r="B471" s="3" t="s">
         <v>459</v>
@@ -9144,7 +9145,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="472" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A472" s="3"/>
       <c r="B472" s="3" t="s">
         <v>457</v>
@@ -9156,7 +9157,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="473" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A473" s="3"/>
       <c r="B473" s="3" t="s">
         <v>455</v>
@@ -9168,7 +9169,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="474" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A474" s="3"/>
       <c r="B474" s="3" t="s">
         <v>454</v>
@@ -9180,7 +9181,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="475" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A475" s="3"/>
       <c r="B475" s="3" t="s">
         <v>452</v>
@@ -9192,7 +9193,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="476" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A476" s="3"/>
       <c r="B476" s="3" t="s">
         <v>450</v>
@@ -9204,7 +9205,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="477" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A477" s="3"/>
       <c r="B477" s="3" t="s">
         <v>448</v>
@@ -9216,7 +9217,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="478" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A478" s="3"/>
       <c r="B478" s="3" t="s">
         <v>446</v>
@@ -9228,7 +9229,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="479" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A479" s="3"/>
       <c r="B479" s="3" t="s">
         <v>444</v>
@@ -9240,7 +9241,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="480" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A480" s="3"/>
       <c r="B480" s="3" t="s">
         <v>442</v>
@@ -9252,7 +9253,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="481" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A481" s="3"/>
       <c r="B481" s="3" t="s">
         <v>441</v>
@@ -9264,7 +9265,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="482" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A482" s="3"/>
       <c r="B482" s="3" t="s">
         <v>439</v>
@@ -9276,7 +9277,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="483" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A483" s="1" t="s">
         <v>156</v>
       </c>
@@ -9304,7 +9305,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="485" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A485" s="1" t="s">
         <v>156</v>
       </c>
@@ -9318,7 +9319,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="486" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A486" s="3"/>
       <c r="B486" s="3" t="s">
         <v>433</v>
@@ -9330,7 +9331,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="487" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A487" s="3"/>
       <c r="B487" s="3" t="s">
         <v>431</v>
@@ -9342,7 +9343,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="488" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A488" s="3"/>
       <c r="B488" s="3" t="s">
         <v>430</v>
@@ -9354,7 +9355,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="489" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A489" s="3"/>
       <c r="B489" s="3" t="s">
         <v>428</v>
@@ -9366,7 +9367,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="490" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A490" s="3"/>
       <c r="B490" s="3" t="s">
         <v>426</v>
@@ -9378,7 +9379,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="491" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A491" s="3"/>
       <c r="B491" s="3" t="s">
         <v>424</v>
@@ -9390,7 +9391,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="492" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A492" s="3"/>
       <c r="B492" s="3" t="s">
         <v>422</v>
@@ -9402,7 +9403,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="493" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A493" s="3"/>
       <c r="B493" s="3" t="s">
         <v>420</v>
@@ -9414,7 +9415,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="494" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A494" s="3"/>
       <c r="B494" s="3" t="s">
         <v>418</v>
@@ -9426,7 +9427,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="495" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A495" s="3"/>
       <c r="B495" s="3" t="s">
         <v>416</v>
@@ -9438,7 +9439,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="496" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A496" s="3"/>
       <c r="B496" s="3" t="s">
         <v>414</v>
@@ -9450,7 +9451,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="497" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A497" s="1" t="s">
         <v>156</v>
       </c>
@@ -9464,7 +9465,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="498" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A498" s="1" t="s">
         <v>156</v>
       </c>
@@ -9478,7 +9479,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="499" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A499" s="3"/>
       <c r="B499" s="3" t="s">
         <v>408</v>
@@ -9490,7 +9491,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="500" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A500" s="3"/>
       <c r="B500" s="3" t="s">
         <v>406</v>
@@ -9502,7 +9503,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="501" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A501" s="3"/>
       <c r="B501" s="3" t="s">
         <v>404</v>
@@ -9514,7 +9515,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="502" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A502" s="3"/>
       <c r="B502" s="3" t="s">
         <v>402</v>
@@ -9526,7 +9527,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="503" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A503" s="3"/>
       <c r="B503" s="3" t="s">
         <v>400</v>
@@ -9538,7 +9539,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="504" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A504" s="3"/>
       <c r="B504" s="3" t="s">
         <v>398</v>
@@ -9550,7 +9551,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="505" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A505" s="3"/>
       <c r="B505" s="3" t="s">
         <v>396</v>
@@ -9562,7 +9563,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="506" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A506" s="3"/>
       <c r="B506" s="3" t="s">
         <v>394</v>
@@ -9574,7 +9575,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="507" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A507" s="3"/>
       <c r="B507" s="3" t="s">
         <v>393</v>
@@ -9586,7 +9587,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="508" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A508" s="3"/>
       <c r="B508" s="3" t="s">
         <v>391</v>
@@ -9598,7 +9599,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="509" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A509" s="3" t="s">
         <v>972</v>
       </c>
@@ -9612,7 +9613,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="510" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A510" s="3"/>
       <c r="B510" s="3" t="s">
         <v>387</v>
@@ -9624,7 +9625,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="511" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A511" s="3"/>
       <c r="B511" s="3" t="s">
         <v>386</v>
@@ -9636,7 +9637,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="512" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A512" s="3"/>
       <c r="B512" s="3" t="s">
         <v>384</v>
@@ -9648,7 +9649,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="513" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A513" s="3"/>
       <c r="B513" s="3" t="s">
         <v>382</v>
@@ -9660,7 +9661,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="514" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A514" s="3"/>
       <c r="B514" s="3" t="s">
         <v>380</v>
@@ -9672,7 +9673,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="515" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A515" s="3"/>
       <c r="B515" s="3" t="s">
         <v>378</v>
@@ -9684,7 +9685,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="516" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A516" s="3"/>
       <c r="B516" s="3" t="s">
         <v>376</v>
@@ -9696,7 +9697,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="517" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A517" s="3" t="s">
         <v>972</v>
       </c>
@@ -9710,7 +9711,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="518" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A518" s="3"/>
       <c r="B518" s="3" t="s">
         <v>372</v>
@@ -9722,7 +9723,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="519" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A519" s="3"/>
       <c r="B519" s="3" t="s">
         <v>370</v>
@@ -9734,7 +9735,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="520" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A520" s="3" t="s">
         <v>972</v>
       </c>
@@ -9748,7 +9749,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="521" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A521" s="3" t="s">
         <v>972</v>
       </c>
@@ -9762,7 +9763,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="522" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A522" s="3"/>
       <c r="B522" s="3" t="s">
         <v>364</v>
@@ -9774,8 +9775,15 @@
         <v>363</v>
       </c>
     </row>
+    <row r="523" spans="1:6" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="A1:F523"/>
+  <autoFilter ref="A1:F523">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Shows-e-Eventos;"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:F200">
     <sortCondition ref="A2:A200"/>
     <sortCondition ref="C2:C200"/>

</xml_diff>